<commit_message>
rest of code and data
</commit_message>
<xml_diff>
--- a/data/graphData/all_bot75.xlsx
+++ b/data/graphData/all_bot75.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cindy\Documents\viz\trial2\data1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cindy\Documents\misinformationTrump\data\graphData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7703111-96B9-4E30-AEF1-3ABCDD307040}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCC277E-A6D8-47FC-BF96-A7FBA33F57B0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_bot75" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -509,9 +512,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -866,10 +871,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3380"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B3402"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A3389" workbookViewId="0">
+      <selection activeCell="A3403" sqref="A3403"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
@@ -27913,6 +27920,116 @@
         <v>876</v>
       </c>
     </row>
+    <row r="3381" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3381" s="2">
+        <v>3.6111111111111114E-3</v>
+      </c>
+    </row>
+    <row r="3382" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3382" s="2">
+        <v>2.0381944444444446E-2</v>
+      </c>
+    </row>
+    <row r="3383" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3383" s="2">
+        <v>2.0879629629629626E-2</v>
+      </c>
+    </row>
+    <row r="3384" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3384" s="2">
+        <v>2.8749999999999998E-2</v>
+      </c>
+    </row>
+    <row r="3385" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3385" s="2">
+        <v>3.6851851851851851E-2</v>
+      </c>
+    </row>
+    <row r="3386" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3386" s="2">
+        <v>4.8472222222222222E-2</v>
+      </c>
+    </row>
+    <row r="3387" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3387" s="2">
+        <v>7.300925925925926E-2</v>
+      </c>
+    </row>
+    <row r="3388" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3388" s="2">
+        <v>9.4953703703703707E-2</v>
+      </c>
+    </row>
+    <row r="3389" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3389" s="2">
+        <v>0.10130787037037037</v>
+      </c>
+    </row>
+    <row r="3390" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3390" s="2">
+        <v>0.12807870370370369</v>
+      </c>
+    </row>
+    <row r="3391" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3391" s="3">
+        <v>2.6504629629629625E-3</v>
+      </c>
+    </row>
+    <row r="3392" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3392" s="3">
+        <v>7.3495370370370372E-3</v>
+      </c>
+    </row>
+    <row r="3393" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3393" s="3">
+        <v>8.1018518518518514E-3</v>
+      </c>
+    </row>
+    <row r="3394" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3394" s="3">
+        <v>8.4837962962962966E-3</v>
+      </c>
+    </row>
+    <row r="3395" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3395" s="3">
+        <v>1.045138888888889E-2</v>
+      </c>
+    </row>
+    <row r="3396" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3396" s="3">
+        <v>1.6863425925925928E-2</v>
+      </c>
+    </row>
+    <row r="3397" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3397" s="3">
+        <v>3.0011574074074076E-2</v>
+      </c>
+    </row>
+    <row r="3398" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3398" s="3">
+        <v>3.8935185185185191E-2</v>
+      </c>
+    </row>
+    <row r="3399" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3399" s="3">
+        <v>5.3414351851851859E-2</v>
+      </c>
+    </row>
+    <row r="3400" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3400" s="3">
+        <v>7.5682870370370373E-2</v>
+      </c>
+    </row>
+    <row r="3401" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3401" s="3">
+        <v>9.0752314814814813E-2</v>
+      </c>
+    </row>
+    <row r="3402" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3402" s="3">
+        <v>9.3865740740740736E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>